<commit_message>
updated printff function to represent text better in terminal
</commit_message>
<xml_diff>
--- a/team_file.xlsx
+++ b/team_file.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:L136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2549,168 +2549,2156 @@
     </row>
     <row r="67"/>
     <row r="68">
-      <c r="A68" s="3" t="inlineStr">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2021/01/04</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>2021/01/04</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2021/01/05</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>2021/01/05</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2021/01/06</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>2021/01/06</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2021/01/10</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>2021/01/10</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2021/01/11</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>2021/01/11</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2021/01/12</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>2021/01/12</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2021/01/16</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>2021/01/16</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2021/01/17</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>2021/01/17</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2021/01/18</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>2021/01/18</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2021/01/22</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>2021/01/22</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2021/01/23</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>2021/01/23</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2021/01/24</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>2021/01/24</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2021/01/28</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>2021/01/28</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2021/01/29</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>2021/01/29</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2021/01/30</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>2021/01/30</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="83"/>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2021/01/01</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>2021/01/01</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2021/01/02</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>2021/01/02</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2021/01/03</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>2021/01/03</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>2021/01/07</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>2021/01/07</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2021/01/08</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>2021/01/08</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>2021/01/09</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>2021/01/09</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>2021/01/13</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>2021/01/13</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>2021/01/14</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>2021/01/14</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>2021/01/15</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>2021/01/15</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>2021/01/19</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>2021/01/19</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>2021/01/20</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>2021/01/20</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>2021/01/21</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>2021/01/21</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>2021/01/25</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>2021/01/25</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>2021/01/26</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>2021/01/26</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>2021/01/27</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>2021/01/27</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>2021/01/31</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>2021/01/31</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="100"/>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>2021/01/04</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>2021/01/04</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>2021/01/05</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>2021/01/05</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>2021/01/06</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>2021/01/06</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>2021/01/10</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>2021/01/10</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>2021/01/11</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>2021/01/11</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>2021/01/12</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>2021/01/12</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>2021/01/16</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>2021/01/16</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>2021/01/17</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>2021/01/17</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>2021/01/18</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>2021/01/18</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>2021/01/22</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>2021/01/22</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>2021/01/23</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>2021/01/23</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>2021/01/24</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>2021/01/24</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>2021/01/28</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>2021/01/28</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>2021/01/29</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>2021/01/29</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>2021/01/30</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>2021/01/30</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="116"/>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>2021/01/01</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>2021/01/01</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>2021/01/02</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>2021/01/02</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>2021/01/03</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>2021/01/03</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>2021/01/07</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>2021/01/07</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>2021/01/08</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>2021/01/08</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>2021/01/09</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>2021/01/09</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>2021/01/13</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>2021/01/13</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>2021/01/14</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>2021/01/14</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>2021/01/15</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>2021/01/15</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>2021/01/19</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>2021/01/19</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>2021/01/20</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>2021/01/20</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>2021/01/21</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>2021/01/21</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>2021/01/25</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>2021/01/25</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>2021/01/26</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>2021/01/26</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>2021/01/27</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>2021/01/27</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>2021/01/31</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>2021/01/31</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="133"/>
+    <row r="134">
+      <c r="A134" s="3" t="inlineStr">
         <is>
           <t>Person1</t>
         </is>
       </c>
-      <c r="B68" s="3" t="inlineStr">
+      <c r="B134" s="3" t="inlineStr">
         <is>
           <t>someone1@example.com</t>
         </is>
       </c>
-      <c r="C68" s="3" t="inlineStr">
+      <c r="C134" s="3" t="inlineStr">
         <is>
           <t>Manager</t>
         </is>
       </c>
-      <c r="D68" s="5" t="inlineStr">
+      <c r="D134" s="5" t="inlineStr">
         <is>
           <t>1/1/2021</t>
         </is>
       </c>
-      <c r="E68" s="3" t="inlineStr">
+      <c r="E134" s="3" t="inlineStr">
         <is>
           <t>10am</t>
         </is>
       </c>
-      <c r="F68" s="5" t="inlineStr">
+      <c r="F134" s="5" t="inlineStr">
         <is>
           <t>1/1/2021</t>
         </is>
       </c>
-      <c r="G68" s="3" t="inlineStr">
+      <c r="G134" s="3" t="inlineStr">
         <is>
           <t>6pm</t>
         </is>
       </c>
-      <c r="H68" s="3" t="inlineStr">
+      <c r="H134" s="3" t="inlineStr">
         <is>
           <t>1. White</t>
         </is>
       </c>
-      <c r="I68" s="3" t="n"/>
-      <c r="J68" s="3" t="n">
+      <c r="I134" s="3" t="n"/>
+      <c r="J134" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="K68" s="3" t="inlineStr">
+      <c r="K134" s="3" t="inlineStr">
         <is>
           <t>Stock opening</t>
         </is>
       </c>
-      <c r="L68" s="3" t="inlineStr">
+      <c r="L134" s="3" t="inlineStr">
         <is>
           <t>1. Shared</t>
         </is>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" s="3" t="inlineStr">
+    <row r="135">
+      <c r="A135" s="3" t="inlineStr">
         <is>
           <t>Person2</t>
         </is>
       </c>
-      <c r="B69" s="3" t="inlineStr">
+      <c r="B135" s="3" t="inlineStr">
         <is>
           <t>someone2@example.com</t>
         </is>
       </c>
-      <c r="C69" s="3" t="inlineStr">
+      <c r="C135" s="3" t="inlineStr">
         <is>
           <t>Sales</t>
         </is>
       </c>
-      <c r="D69" s="5" t="inlineStr">
+      <c r="D135" s="5" t="inlineStr">
         <is>
           <t>1/1/2021</t>
         </is>
       </c>
-      <c r="E69" s="3" t="inlineStr">
+      <c r="E135" s="3" t="inlineStr">
         <is>
           <t>11:00</t>
         </is>
       </c>
-      <c r="F69" s="5" t="inlineStr">
+      <c r="F135" s="5" t="inlineStr">
         <is>
           <t>1/1/2021</t>
         </is>
       </c>
-      <c r="G69" s="3" t="inlineStr">
+      <c r="G135" s="3" t="inlineStr">
         <is>
           <t>18:00</t>
         </is>
       </c>
-      <c r="H69" s="3" t="inlineStr">
+      <c r="H135" s="3" t="inlineStr">
         <is>
           <t>1. White</t>
         </is>
       </c>
-      <c r="I69" s="3" t="n"/>
-      <c r="J69" s="3" t="n">
+      <c r="I135" s="3" t="n"/>
+      <c r="J135" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="K69" s="3" t="inlineStr">
+      <c r="K135" s="3" t="inlineStr">
         <is>
           <t>Match sales report</t>
         </is>
       </c>
-      <c r="L69" s="3" t="inlineStr">
+      <c r="L135" s="3" t="inlineStr">
         <is>
           <t>1. Shared</t>
         </is>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" s="3" t="inlineStr">
+    <row r="136">
+      <c r="A136" s="3" t="inlineStr">
         <is>
           <t>Person3</t>
         </is>
       </c>
-      <c r="B70" s="3" t="inlineStr">
+      <c r="B136" s="3" t="inlineStr">
         <is>
           <t>someone3@example.com</t>
         </is>
       </c>
-      <c r="C70" s="3" t="inlineStr">
+      <c r="C136" s="3" t="inlineStr">
         <is>
           <t>Manager</t>
         </is>
       </c>
-      <c r="D70" s="5" t="inlineStr">
+      <c r="D136" s="5" t="inlineStr">
         <is>
           <t>1/1/2021</t>
         </is>
       </c>
-      <c r="E70" s="3" t="inlineStr">
+      <c r="E136" s="3" t="inlineStr">
         <is>
           <t>10:00</t>
         </is>
       </c>
-      <c r="F70" s="5" t="inlineStr">
+      <c r="F136" s="5" t="inlineStr">
         <is>
           <t>1/1/2021</t>
         </is>
       </c>
-      <c r="G70" s="3" t="inlineStr">
+      <c r="G136" s="3" t="inlineStr">
         <is>
           <t>6pm</t>
         </is>
       </c>
-      <c r="H70" s="3" t="inlineStr">
+      <c r="H136" s="3" t="inlineStr">
         <is>
           <t>1. White</t>
         </is>
       </c>
-      <c r="I70" s="3" t="n"/>
-      <c r="J70" s="3" t="n">
+      <c r="I136" s="3" t="n"/>
+      <c r="J136" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K70" s="3" t="inlineStr">
+      <c r="K136" s="3" t="inlineStr">
         <is>
           <t>Stock opening</t>
         </is>
       </c>
-      <c r="L70" s="3" t="inlineStr">
+      <c r="L136" s="3" t="inlineStr">
         <is>
           <t>1. Shared</t>
         </is>

</xml_diff>

<commit_message>
recompiled program without terminal at the background
</commit_message>
<xml_diff>
--- a/team_file.xlsx
+++ b/team_file.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instructions" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Shifts" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Day Notes" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Members" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Instructions" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Shifts" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Day Notes" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Members" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="m/d/yyyy" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -70,67 +70,67 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -494,23 +494,23 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="2:67 A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="2:67 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.70703125" defaultRowHeight="14.4" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="8" width="200.01"/>
+    <col width="200.01" customWidth="1" style="8" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="14.4" r="1" s="9">
+    <row r="1" ht="14.4" customHeight="1" s="9">
       <c r="A1" s="10" t="inlineStr">
         <is>
           <t>Instructions</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="158.4" r="2" s="9">
+    <row r="2" ht="158.4" customHeight="1" s="9">
       <c r="A2" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">
@@ -528,9 +528,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
@@ -540,29 +540,29 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L652"/>
+  <dimension ref="A1:L718"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A61" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A67" activeCellId="0" pane="topLeft" sqref="2:67"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A67" activeCellId="0" sqref="2:67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.70703125" defaultRowHeight="14.4" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="8" width="9.130000000000001"/>
-    <col customWidth="1" max="2" min="2" style="8" width="24.34"/>
-    <col customWidth="1" max="3" min="3" style="8" width="9.33"/>
-    <col customWidth="1" max="4" min="4" style="8" width="15.11"/>
-    <col customWidth="1" max="5" min="5" style="8" width="15.34"/>
-    <col customWidth="1" max="6" min="6" style="8" width="14.11"/>
-    <col customWidth="1" max="7" min="7" style="8" width="14.35"/>
-    <col customWidth="1" max="8" min="8" style="8" width="12.66"/>
-    <col customWidth="1" max="9" min="9" style="8" width="13.22"/>
-    <col customWidth="1" max="10" min="10" style="8" width="22.11"/>
-    <col customWidth="1" max="11" min="11" style="8" width="17.89"/>
-    <col customWidth="1" max="12" min="12" style="8" width="9.66"/>
+    <col width="9.130000000000001" customWidth="1" style="8" min="1" max="1"/>
+    <col width="24.34" customWidth="1" style="8" min="2" max="2"/>
+    <col width="9.33" customWidth="1" style="8" min="3" max="3"/>
+    <col width="15.11" customWidth="1" style="8" min="4" max="4"/>
+    <col width="15.34" customWidth="1" style="8" min="5" max="5"/>
+    <col width="14.11" customWidth="1" style="8" min="6" max="6"/>
+    <col width="14.35" customWidth="1" style="8" min="7" max="7"/>
+    <col width="12.66" customWidth="1" style="8" min="8" max="8"/>
+    <col width="13.22" customWidth="1" style="8" min="9" max="9"/>
+    <col width="22.11" customWidth="1" style="8" min="10" max="10"/>
+    <col width="17.89" customWidth="1" style="8" min="11" max="11"/>
+    <col width="9.66" customWidth="1" style="8" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="14.4" r="1" s="9">
+    <row r="1" ht="14.4" customHeight="1" s="9">
       <c r="A1" s="11" t="inlineStr">
         <is>
           <t>Member</t>
@@ -624,7 +624,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="2" s="9">
+    <row r="2" ht="13.8" customHeight="1" s="9">
       <c r="A2" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -661,7 +661,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="3" s="9">
+    <row r="3" ht="13.8" customHeight="1" s="9">
       <c r="A3" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -698,7 +698,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="4" s="9">
+    <row r="4" ht="13.8" customHeight="1" s="9">
       <c r="A4" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -735,7 +735,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="5" s="9">
+    <row r="5" ht="13.8" customHeight="1" s="9">
       <c r="A5" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -772,7 +772,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="6" s="9">
+    <row r="6" ht="13.8" customHeight="1" s="9">
       <c r="A6" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -809,7 +809,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="7" s="9">
+    <row r="7" ht="13.8" customHeight="1" s="9">
       <c r="A7" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -846,7 +846,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="8" s="9">
+    <row r="8" ht="13.8" customHeight="1" s="9">
       <c r="A8" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -883,7 +883,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="9" s="9">
+    <row r="9" ht="13.8" customHeight="1" s="9">
       <c r="A9" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -920,7 +920,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="10" s="9">
+    <row r="10" ht="13.8" customHeight="1" s="9">
       <c r="A10" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -957,7 +957,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="11" s="9">
+    <row r="11" ht="13.8" customHeight="1" s="9">
       <c r="A11" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -994,7 +994,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="12" s="9">
+    <row r="12" ht="13.8" customHeight="1" s="9">
       <c r="A12" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -1031,7 +1031,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="13" s="9">
+    <row r="13" ht="13.8" customHeight="1" s="9">
       <c r="A13" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -1068,7 +1068,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="14" s="9">
+    <row r="14" ht="13.8" customHeight="1" s="9">
       <c r="A14" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -1105,7 +1105,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="15" s="9">
+    <row r="15" ht="13.8" customHeight="1" s="9">
       <c r="A15" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -1142,7 +1142,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="16" s="9">
+    <row r="16" ht="13.8" customHeight="1" s="9">
       <c r="A16" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -1179,8 +1179,8 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="17" s="9"/>
-    <row customHeight="1" ht="13.8" r="18" s="9">
+    <row r="17" ht="13.8" customHeight="1" s="9"/>
+    <row r="18" ht="13.8" customHeight="1" s="9">
       <c r="A18" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1217,7 +1217,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="19" s="9">
+    <row r="19" ht="13.8" customHeight="1" s="9">
       <c r="A19" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1254,7 +1254,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="20" s="9">
+    <row r="20" ht="13.8" customHeight="1" s="9">
       <c r="A20" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1291,7 +1291,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="21" s="9">
+    <row r="21" ht="13.8" customHeight="1" s="9">
       <c r="A21" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1328,7 +1328,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="22" s="9">
+    <row r="22" ht="13.8" customHeight="1" s="9">
       <c r="A22" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1365,7 +1365,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="23" s="9">
+    <row r="23" ht="13.8" customHeight="1" s="9">
       <c r="A23" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1402,7 +1402,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="24" s="9">
+    <row r="24" ht="13.8" customHeight="1" s="9">
       <c r="A24" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1439,7 +1439,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="25" s="9">
+    <row r="25" ht="13.8" customHeight="1" s="9">
       <c r="A25" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1476,7 +1476,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="26" s="9">
+    <row r="26" ht="13.8" customHeight="1" s="9">
       <c r="A26" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1513,7 +1513,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="27" s="9">
+    <row r="27" ht="13.8" customHeight="1" s="9">
       <c r="A27" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1550,7 +1550,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="28" s="9">
+    <row r="28" ht="13.8" customHeight="1" s="9">
       <c r="A28" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1587,7 +1587,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="29" s="9">
+    <row r="29" ht="13.8" customHeight="1" s="9">
       <c r="A29" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1624,7 +1624,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="30" s="9">
+    <row r="30" ht="13.8" customHeight="1" s="9">
       <c r="A30" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1661,7 +1661,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="31" s="9">
+    <row r="31" ht="13.8" customHeight="1" s="9">
       <c r="A31" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1698,7 +1698,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="32" s="9">
+    <row r="32" ht="13.8" customHeight="1" s="9">
       <c r="A32" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1735,7 +1735,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="33" s="9">
+    <row r="33" ht="13.8" customHeight="1" s="9">
       <c r="A33" t="inlineStr">
         <is>
           <t>Anastasia Ioseiani</t>
@@ -1772,8 +1772,8 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="34" s="9"/>
-    <row customHeight="1" ht="13.8" r="35" s="9">
+    <row r="34" ht="13.8" customHeight="1" s="9"/>
+    <row r="35" ht="13.8" customHeight="1" s="9">
       <c r="A35" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -1810,7 +1810,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="36" s="9">
+    <row r="36" ht="13.8" customHeight="1" s="9">
       <c r="A36" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -1847,7 +1847,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="37" s="9">
+    <row r="37" ht="13.8" customHeight="1" s="9">
       <c r="A37" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -1884,7 +1884,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="38" s="9">
+    <row r="38" ht="13.8" customHeight="1" s="9">
       <c r="A38" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -1921,7 +1921,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="39" s="9">
+    <row r="39" ht="13.8" customHeight="1" s="9">
       <c r="A39" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -1958,7 +1958,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="40" s="9">
+    <row r="40" ht="13.8" customHeight="1" s="9">
       <c r="A40" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -1995,7 +1995,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="41" s="9">
+    <row r="41" ht="13.8" customHeight="1" s="9">
       <c r="A41" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -2032,7 +2032,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="42" s="9">
+    <row r="42" ht="13.8" customHeight="1" s="9">
       <c r="A42" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -2069,7 +2069,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="43" s="9">
+    <row r="43" ht="13.8" customHeight="1" s="9">
       <c r="A43" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -2106,7 +2106,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="44" s="9">
+    <row r="44" ht="13.8" customHeight="1" s="9">
       <c r="A44" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -2143,7 +2143,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="45" s="9">
+    <row r="45" ht="13.8" customHeight="1" s="9">
       <c r="A45" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -2180,7 +2180,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="46" s="9">
+    <row r="46" ht="13.8" customHeight="1" s="9">
       <c r="A46" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -2217,7 +2217,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="47" s="9">
+    <row r="47" ht="13.8" customHeight="1" s="9">
       <c r="A47" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -2254,7 +2254,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="48" s="9">
+    <row r="48" ht="13.8" customHeight="1" s="9">
       <c r="A48" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -2291,7 +2291,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="49" s="9">
+    <row r="49" ht="13.8" customHeight="1" s="9">
       <c r="A49" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -2328,8 +2328,8 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="50" s="9"/>
-    <row customHeight="1" ht="13.8" r="51" s="9">
+    <row r="50" ht="13.8" customHeight="1" s="9"/>
+    <row r="51" ht="13.8" customHeight="1" s="9">
       <c r="A51" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2366,7 +2366,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="52" s="9">
+    <row r="52" ht="13.8" customHeight="1" s="9">
       <c r="A52" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2403,7 +2403,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="53" s="9">
+    <row r="53" ht="13.8" customHeight="1" s="9">
       <c r="A53" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2440,7 +2440,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="54" s="9">
+    <row r="54" ht="13.8" customHeight="1" s="9">
       <c r="A54" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2477,7 +2477,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="55" s="9">
+    <row r="55" ht="13.8" customHeight="1" s="9">
       <c r="A55" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2514,7 +2514,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="56" s="9">
+    <row r="56" ht="13.8" customHeight="1" s="9">
       <c r="A56" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2551,7 +2551,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="57" s="9">
+    <row r="57" ht="13.8" customHeight="1" s="9">
       <c r="A57" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2588,7 +2588,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="58" s="9">
+    <row r="58" ht="13.8" customHeight="1" s="9">
       <c r="A58" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2625,7 +2625,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="59" s="9">
+    <row r="59" ht="13.8" customHeight="1" s="9">
       <c r="A59" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2662,7 +2662,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="60" s="9">
+    <row r="60" ht="13.8" customHeight="1" s="9">
       <c r="A60" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2699,7 +2699,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="61" s="9">
+    <row r="61" ht="13.8" customHeight="1" s="9">
       <c r="A61" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2736,7 +2736,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="62" s="9">
+    <row r="62" ht="13.8" customHeight="1" s="9">
       <c r="A62" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2773,7 +2773,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="63" s="9">
+    <row r="63" ht="13.8" customHeight="1" s="9">
       <c r="A63" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2810,7 +2810,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="64" s="9">
+    <row r="64" ht="13.8" customHeight="1" s="9">
       <c r="A64" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2847,7 +2847,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="65" s="9">
+    <row r="65" ht="13.8" customHeight="1" s="9">
       <c r="A65" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2884,7 +2884,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="66" s="9">
+    <row r="66" ht="13.8" customHeight="1" s="9">
       <c r="A66" t="inlineStr">
         <is>
           <t>Tamar Khardziani</t>
@@ -2921,7 +2921,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="67" s="9"/>
+    <row r="67" ht="13.8" customHeight="1" s="9"/>
     <row r="68">
       <c r="A68" s="8" t="inlineStr">
         <is>
@@ -7518,71 +7518,2303 @@
       </c>
     </row>
     <row r="199"/>
-    <row r="200"/>
-    <row r="201"/>
-    <row r="202"/>
-    <row r="203"/>
-    <row r="204"/>
-    <row r="205"/>
-    <row r="206"/>
-    <row r="207"/>
-    <row r="208"/>
-    <row r="209"/>
-    <row r="210"/>
-    <row r="211"/>
-    <row r="212"/>
-    <row r="213"/>
-    <row r="214"/>
+    <row r="200">
+      <c r="A200" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B200" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D200" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/04</t>
+        </is>
+      </c>
+      <c r="E200" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F200" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/04</t>
+        </is>
+      </c>
+      <c r="G200" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H200" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B201" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D201" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/05</t>
+        </is>
+      </c>
+      <c r="E201" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F201" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/05</t>
+        </is>
+      </c>
+      <c r="G201" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H201" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B202" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D202" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/06</t>
+        </is>
+      </c>
+      <c r="E202" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F202" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/06</t>
+        </is>
+      </c>
+      <c r="G202" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H202" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B203" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D203" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/10</t>
+        </is>
+      </c>
+      <c r="E203" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F203" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/10</t>
+        </is>
+      </c>
+      <c r="G203" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H203" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B204" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D204" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/11</t>
+        </is>
+      </c>
+      <c r="E204" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F204" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/11</t>
+        </is>
+      </c>
+      <c r="G204" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H204" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B205" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D205" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/12</t>
+        </is>
+      </c>
+      <c r="E205" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F205" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/12</t>
+        </is>
+      </c>
+      <c r="G205" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H205" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B206" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D206" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/16</t>
+        </is>
+      </c>
+      <c r="E206" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F206" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/16</t>
+        </is>
+      </c>
+      <c r="G206" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H206" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B207" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D207" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/17</t>
+        </is>
+      </c>
+      <c r="E207" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F207" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/17</t>
+        </is>
+      </c>
+      <c r="G207" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H207" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B208" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D208" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/18</t>
+        </is>
+      </c>
+      <c r="E208" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F208" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/18</t>
+        </is>
+      </c>
+      <c r="G208" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H208" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B209" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D209" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/22</t>
+        </is>
+      </c>
+      <c r="E209" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F209" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/22</t>
+        </is>
+      </c>
+      <c r="G209" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H209" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B210" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D210" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/23</t>
+        </is>
+      </c>
+      <c r="E210" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F210" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/23</t>
+        </is>
+      </c>
+      <c r="G210" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H210" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B211" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D211" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/24</t>
+        </is>
+      </c>
+      <c r="E211" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F211" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/24</t>
+        </is>
+      </c>
+      <c r="G211" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H211" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B212" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D212" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/28</t>
+        </is>
+      </c>
+      <c r="E212" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F212" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/28</t>
+        </is>
+      </c>
+      <c r="G212" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H212" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B213" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D213" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/29</t>
+        </is>
+      </c>
+      <c r="E213" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F213" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/29</t>
+        </is>
+      </c>
+      <c r="G213" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H213" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="8" t="inlineStr">
+        <is>
+          <t>Nodar Gelovani</t>
+        </is>
+      </c>
+      <c r="B214" s="8" t="inlineStr">
+        <is>
+          <t>ngelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D214" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/30</t>
+        </is>
+      </c>
+      <c r="E214" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F214" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/30</t>
+        </is>
+      </c>
+      <c r="G214" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H214" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
     <row r="215"/>
-    <row r="216"/>
-    <row r="217"/>
-    <row r="218"/>
-    <row r="219"/>
-    <row r="220"/>
-    <row r="221"/>
-    <row r="222"/>
-    <row r="223"/>
-    <row r="224"/>
-    <row r="225"/>
-    <row r="226"/>
-    <row r="227"/>
-    <row r="228"/>
-    <row r="229"/>
-    <row r="230"/>
-    <row r="231"/>
+    <row r="216">
+      <c r="A216" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B216" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D216" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/01</t>
+        </is>
+      </c>
+      <c r="E216" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F216" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/01</t>
+        </is>
+      </c>
+      <c r="G216" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H216" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B217" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D217" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/02</t>
+        </is>
+      </c>
+      <c r="E217" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F217" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/02</t>
+        </is>
+      </c>
+      <c r="G217" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H217" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B218" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D218" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/03</t>
+        </is>
+      </c>
+      <c r="E218" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F218" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/03</t>
+        </is>
+      </c>
+      <c r="G218" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H218" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B219" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D219" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/07</t>
+        </is>
+      </c>
+      <c r="E219" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F219" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/07</t>
+        </is>
+      </c>
+      <c r="G219" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H219" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B220" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D220" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/08</t>
+        </is>
+      </c>
+      <c r="E220" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F220" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/08</t>
+        </is>
+      </c>
+      <c r="G220" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H220" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B221" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D221" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/09</t>
+        </is>
+      </c>
+      <c r="E221" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F221" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/09</t>
+        </is>
+      </c>
+      <c r="G221" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H221" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B222" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D222" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/13</t>
+        </is>
+      </c>
+      <c r="E222" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F222" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/13</t>
+        </is>
+      </c>
+      <c r="G222" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H222" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B223" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D223" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/14</t>
+        </is>
+      </c>
+      <c r="E223" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F223" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/14</t>
+        </is>
+      </c>
+      <c r="G223" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H223" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B224" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D224" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/15</t>
+        </is>
+      </c>
+      <c r="E224" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F224" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/15</t>
+        </is>
+      </c>
+      <c r="G224" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H224" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B225" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D225" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/19</t>
+        </is>
+      </c>
+      <c r="E225" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F225" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/19</t>
+        </is>
+      </c>
+      <c r="G225" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H225" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B226" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D226" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/20</t>
+        </is>
+      </c>
+      <c r="E226" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F226" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/20</t>
+        </is>
+      </c>
+      <c r="G226" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H226" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B227" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D227" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/21</t>
+        </is>
+      </c>
+      <c r="E227" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F227" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/21</t>
+        </is>
+      </c>
+      <c r="G227" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H227" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B228" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D228" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/25</t>
+        </is>
+      </c>
+      <c r="E228" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F228" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/25</t>
+        </is>
+      </c>
+      <c r="G228" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H228" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B229" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D229" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/26</t>
+        </is>
+      </c>
+      <c r="E229" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F229" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/26</t>
+        </is>
+      </c>
+      <c r="G229" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H229" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B230" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D230" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/27</t>
+        </is>
+      </c>
+      <c r="E230" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F230" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/27</t>
+        </is>
+      </c>
+      <c r="G230" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H230" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="8" t="inlineStr">
+        <is>
+          <t>Anastasia Ioseiani</t>
+        </is>
+      </c>
+      <c r="B231" s="8" t="inlineStr">
+        <is>
+          <t>aioseliani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D231" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/31</t>
+        </is>
+      </c>
+      <c r="E231" s="8" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F231" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/31</t>
+        </is>
+      </c>
+      <c r="G231" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="H231" s="8" t="inlineStr">
+        <is>
+          <t>5. Pink</t>
+        </is>
+      </c>
+    </row>
     <row r="232"/>
-    <row r="233"/>
-    <row r="234"/>
-    <row r="235"/>
-    <row r="236"/>
-    <row r="237"/>
-    <row r="238"/>
-    <row r="239"/>
-    <row r="240"/>
-    <row r="241"/>
-    <row r="242"/>
-    <row r="243"/>
-    <row r="244"/>
-    <row r="245"/>
-    <row r="246"/>
-    <row r="247"/>
+    <row r="233">
+      <c r="A233" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B233" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D233" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/04</t>
+        </is>
+      </c>
+      <c r="E233" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F233" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/04</t>
+        </is>
+      </c>
+      <c r="G233" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H233" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B234" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D234" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/05</t>
+        </is>
+      </c>
+      <c r="E234" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F234" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/05</t>
+        </is>
+      </c>
+      <c r="G234" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H234" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B235" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D235" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/06</t>
+        </is>
+      </c>
+      <c r="E235" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F235" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/06</t>
+        </is>
+      </c>
+      <c r="G235" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H235" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B236" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D236" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/10</t>
+        </is>
+      </c>
+      <c r="E236" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F236" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/10</t>
+        </is>
+      </c>
+      <c r="G236" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H236" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B237" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D237" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/11</t>
+        </is>
+      </c>
+      <c r="E237" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F237" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/11</t>
+        </is>
+      </c>
+      <c r="G237" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H237" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B238" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D238" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/12</t>
+        </is>
+      </c>
+      <c r="E238" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F238" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/12</t>
+        </is>
+      </c>
+      <c r="G238" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H238" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B239" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D239" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/16</t>
+        </is>
+      </c>
+      <c r="E239" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F239" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/16</t>
+        </is>
+      </c>
+      <c r="G239" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H239" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B240" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D240" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/17</t>
+        </is>
+      </c>
+      <c r="E240" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F240" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/17</t>
+        </is>
+      </c>
+      <c r="G240" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H240" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B241" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D241" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/18</t>
+        </is>
+      </c>
+      <c r="E241" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F241" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/18</t>
+        </is>
+      </c>
+      <c r="G241" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H241" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B242" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D242" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/22</t>
+        </is>
+      </c>
+      <c r="E242" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F242" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/22</t>
+        </is>
+      </c>
+      <c r="G242" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H242" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B243" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D243" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/23</t>
+        </is>
+      </c>
+      <c r="E243" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F243" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/23</t>
+        </is>
+      </c>
+      <c r="G243" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H243" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B244" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D244" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/24</t>
+        </is>
+      </c>
+      <c r="E244" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F244" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/24</t>
+        </is>
+      </c>
+      <c r="G244" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H244" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B245" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D245" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/28</t>
+        </is>
+      </c>
+      <c r="E245" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F245" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/28</t>
+        </is>
+      </c>
+      <c r="G245" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H245" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B246" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D246" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/29</t>
+        </is>
+      </c>
+      <c r="E246" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F246" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/29</t>
+        </is>
+      </c>
+      <c r="G246" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H246" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="8" t="inlineStr">
+        <is>
+          <t>Giorgi Gelovani</t>
+        </is>
+      </c>
+      <c r="B247" s="8" t="inlineStr">
+        <is>
+          <t>ggelovani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D247" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/30</t>
+        </is>
+      </c>
+      <c r="E247" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F247" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/30</t>
+        </is>
+      </c>
+      <c r="G247" s="8" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="H247" s="8" t="inlineStr">
+        <is>
+          <t>3. Green</t>
+        </is>
+      </c>
+    </row>
     <row r="248"/>
-    <row r="249"/>
-    <row r="250"/>
-    <row r="251"/>
-    <row r="252"/>
-    <row r="253"/>
-    <row r="254"/>
-    <row r="255"/>
-    <row r="256"/>
-    <row r="257"/>
-    <row r="258"/>
-    <row r="259"/>
-    <row r="260"/>
-    <row r="261"/>
-    <row r="262"/>
-    <row r="263"/>
-    <row r="264"/>
+    <row r="249">
+      <c r="A249" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B249" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D249" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/01</t>
+        </is>
+      </c>
+      <c r="E249" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F249" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/01</t>
+        </is>
+      </c>
+      <c r="G249" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H249" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B250" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D250" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/02</t>
+        </is>
+      </c>
+      <c r="E250" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F250" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/02</t>
+        </is>
+      </c>
+      <c r="G250" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H250" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B251" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D251" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/03</t>
+        </is>
+      </c>
+      <c r="E251" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F251" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/03</t>
+        </is>
+      </c>
+      <c r="G251" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H251" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B252" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D252" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/07</t>
+        </is>
+      </c>
+      <c r="E252" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F252" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/07</t>
+        </is>
+      </c>
+      <c r="G252" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H252" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B253" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D253" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/08</t>
+        </is>
+      </c>
+      <c r="E253" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F253" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/08</t>
+        </is>
+      </c>
+      <c r="G253" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H253" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B254" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D254" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/09</t>
+        </is>
+      </c>
+      <c r="E254" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F254" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/09</t>
+        </is>
+      </c>
+      <c r="G254" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H254" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B255" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D255" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/13</t>
+        </is>
+      </c>
+      <c r="E255" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F255" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/13</t>
+        </is>
+      </c>
+      <c r="G255" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H255" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B256" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D256" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/14</t>
+        </is>
+      </c>
+      <c r="E256" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F256" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/14</t>
+        </is>
+      </c>
+      <c r="G256" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H256" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B257" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D257" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/15</t>
+        </is>
+      </c>
+      <c r="E257" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F257" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/15</t>
+        </is>
+      </c>
+      <c r="G257" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H257" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B258" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D258" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/19</t>
+        </is>
+      </c>
+      <c r="E258" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F258" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/19</t>
+        </is>
+      </c>
+      <c r="G258" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H258" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B259" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D259" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/20</t>
+        </is>
+      </c>
+      <c r="E259" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F259" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/20</t>
+        </is>
+      </c>
+      <c r="G259" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H259" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B260" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D260" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/21</t>
+        </is>
+      </c>
+      <c r="E260" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F260" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/21</t>
+        </is>
+      </c>
+      <c r="G260" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H260" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B261" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D261" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/25</t>
+        </is>
+      </c>
+      <c r="E261" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F261" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/25</t>
+        </is>
+      </c>
+      <c r="G261" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H261" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B262" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D262" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/26</t>
+        </is>
+      </c>
+      <c r="E262" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F262" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/26</t>
+        </is>
+      </c>
+      <c r="G262" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H262" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B263" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D263" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/27</t>
+        </is>
+      </c>
+      <c r="E263" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F263" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/27</t>
+        </is>
+      </c>
+      <c r="G263" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H263" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="8" t="inlineStr">
+        <is>
+          <t>Tamar Khardziani</t>
+        </is>
+      </c>
+      <c r="B264" s="8" t="inlineStr">
+        <is>
+          <t>tkhardziani@evolution.com</t>
+        </is>
+      </c>
+      <c r="D264" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/31</t>
+        </is>
+      </c>
+      <c r="E264" s="8" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="F264" s="8" t="inlineStr">
+        <is>
+          <t>2021/01/31</t>
+        </is>
+      </c>
+      <c r="G264" s="8" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="H264" s="8" t="inlineStr">
+        <is>
+          <t>2. Blue</t>
+        </is>
+      </c>
+    </row>
     <row r="265"/>
     <row r="266"/>
     <row r="267"/>
@@ -7638,9 +9870,9 @@
     <row r="317"/>
     <row r="318"/>
     <row r="319"/>
-    <row customHeight="1" ht="14.4" r="320" s="9"/>
-    <row customHeight="1" ht="14.4" r="321" s="9"/>
-    <row customHeight="1" ht="14.4" r="322" s="9"/>
+    <row r="320" ht="14.4" customHeight="1" s="9"/>
+    <row r="321" ht="14.4" customHeight="1" s="9"/>
+    <row r="322" ht="14.4" customHeight="1" s="9"/>
     <row r="323"/>
     <row r="324"/>
     <row r="325"/>
@@ -7704,9 +9936,9 @@
     <row r="383"/>
     <row r="384"/>
     <row r="385"/>
-    <row customHeight="1" ht="14.4" r="386" s="9"/>
-    <row customHeight="1" ht="14.4" r="387" s="9"/>
-    <row customHeight="1" ht="14.4" r="388" s="9"/>
+    <row r="386" ht="14.4" customHeight="1" s="9"/>
+    <row r="387" ht="14.4" customHeight="1" s="9"/>
+    <row r="388" ht="14.4" customHeight="1" s="9"/>
     <row r="389"/>
     <row r="390"/>
     <row r="391"/>
@@ -7770,9 +10002,9 @@
     <row r="449"/>
     <row r="450"/>
     <row r="451"/>
-    <row customHeight="1" ht="14.4" r="452" s="9"/>
-    <row customHeight="1" ht="14.4" r="453" s="9"/>
-    <row customHeight="1" ht="14.4" r="454" s="9"/>
+    <row r="452" ht="14.4" customHeight="1" s="9"/>
+    <row r="453" ht="14.4" customHeight="1" s="9"/>
+    <row r="454" ht="14.4" customHeight="1" s="9"/>
     <row r="455"/>
     <row r="456"/>
     <row r="457"/>
@@ -7968,62 +10200,128 @@
     <row r="647"/>
     <row r="648"/>
     <row r="649"/>
-    <row r="650">
-      <c r="A650" s="11" t="n"/>
-      <c r="B650" s="11" t="n"/>
-      <c r="C650" s="11" t="n"/>
-      <c r="D650" s="13" t="n"/>
-      <c r="E650" s="11" t="n"/>
-      <c r="F650" s="13" t="n"/>
-      <c r="G650" s="11" t="n"/>
-      <c r="H650" s="11" t="n"/>
-      <c r="I650" s="11" t="n"/>
-      <c r="J650" s="11" t="n"/>
-      <c r="K650" s="11" t="n"/>
-      <c r="L650" s="11" t="n"/>
-    </row>
-    <row r="651">
-      <c r="A651" s="11" t="n"/>
-      <c r="B651" s="11" t="n"/>
-      <c r="C651" s="11" t="n"/>
-      <c r="D651" s="13" t="n"/>
-      <c r="E651" s="11" t="n"/>
-      <c r="F651" s="13" t="n"/>
-      <c r="G651" s="11" t="n"/>
-      <c r="H651" s="11" t="n"/>
-      <c r="I651" s="11" t="n"/>
-      <c r="J651" s="11" t="n"/>
-      <c r="K651" s="11" t="n"/>
-      <c r="L651" s="11" t="n"/>
-    </row>
-    <row r="652">
-      <c r="A652" s="11" t="n"/>
-      <c r="B652" s="11" t="n"/>
-      <c r="C652" s="11" t="n"/>
-      <c r="D652" s="13" t="n"/>
-      <c r="E652" s="11" t="n"/>
-      <c r="F652" s="13" t="n"/>
-      <c r="G652" s="11" t="n"/>
-      <c r="H652" s="11" t="n"/>
-      <c r="I652" s="11" t="n"/>
-      <c r="J652" s="11" t="n"/>
-      <c r="K652" s="11" t="n"/>
-      <c r="L652" s="11" t="n"/>
+    <row r="650"/>
+    <row r="651"/>
+    <row r="652"/>
+    <row r="653"/>
+    <row r="654"/>
+    <row r="655"/>
+    <row r="656"/>
+    <row r="657"/>
+    <row r="658"/>
+    <row r="659"/>
+    <row r="660"/>
+    <row r="661"/>
+    <row r="662"/>
+    <row r="663"/>
+    <row r="664"/>
+    <row r="665"/>
+    <row r="666"/>
+    <row r="667"/>
+    <row r="668"/>
+    <row r="669"/>
+    <row r="670"/>
+    <row r="671"/>
+    <row r="672"/>
+    <row r="673"/>
+    <row r="674"/>
+    <row r="675"/>
+    <row r="676"/>
+    <row r="677"/>
+    <row r="678"/>
+    <row r="679"/>
+    <row r="680"/>
+    <row r="681"/>
+    <row r="682"/>
+    <row r="683"/>
+    <row r="684"/>
+    <row r="685"/>
+    <row r="686"/>
+    <row r="687"/>
+    <row r="688"/>
+    <row r="689"/>
+    <row r="690"/>
+    <row r="691"/>
+    <row r="692"/>
+    <row r="693"/>
+    <row r="694"/>
+    <row r="695"/>
+    <row r="696"/>
+    <row r="697"/>
+    <row r="698"/>
+    <row r="699"/>
+    <row r="700"/>
+    <row r="701"/>
+    <row r="702"/>
+    <row r="703"/>
+    <row r="704"/>
+    <row r="705"/>
+    <row r="706"/>
+    <row r="707"/>
+    <row r="708"/>
+    <row r="709"/>
+    <row r="710"/>
+    <row r="711"/>
+    <row r="712"/>
+    <row r="713"/>
+    <row r="714"/>
+    <row r="715"/>
+    <row r="716">
+      <c r="A716" s="11" t="n"/>
+      <c r="B716" s="11" t="n"/>
+      <c r="C716" s="11" t="n"/>
+      <c r="D716" s="13" t="n"/>
+      <c r="E716" s="11" t="n"/>
+      <c r="F716" s="13" t="n"/>
+      <c r="G716" s="11" t="n"/>
+      <c r="H716" s="11" t="n"/>
+      <c r="I716" s="11" t="n"/>
+      <c r="J716" s="11" t="n"/>
+      <c r="K716" s="11" t="n"/>
+      <c r="L716" s="11" t="n"/>
+    </row>
+    <row r="717">
+      <c r="A717" s="11" t="n"/>
+      <c r="B717" s="11" t="n"/>
+      <c r="C717" s="11" t="n"/>
+      <c r="D717" s="13" t="n"/>
+      <c r="E717" s="11" t="n"/>
+      <c r="F717" s="13" t="n"/>
+      <c r="G717" s="11" t="n"/>
+      <c r="H717" s="11" t="n"/>
+      <c r="I717" s="11" t="n"/>
+      <c r="J717" s="11" t="n"/>
+      <c r="K717" s="11" t="n"/>
+      <c r="L717" s="11" t="n"/>
+    </row>
+    <row r="718">
+      <c r="A718" s="11" t="n"/>
+      <c r="B718" s="11" t="n"/>
+      <c r="C718" s="11" t="n"/>
+      <c r="D718" s="13" t="n"/>
+      <c r="E718" s="11" t="n"/>
+      <c r="F718" s="13" t="n"/>
+      <c r="G718" s="11" t="n"/>
+      <c r="H718" s="11" t="n"/>
+      <c r="I718" s="11" t="n"/>
+      <c r="J718" s="11" t="n"/>
+      <c r="K718" s="11" t="n"/>
+      <c r="L718" s="11" t="n"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="0" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1" sqref="H2:H1001" type="list">
+    <dataValidation sqref="H2:H1001" showErrorMessage="1" showDropDown="0" showInputMessage="1" allowBlank="0" type="list" operator="between">
       <formula1>"1. White,2. Blue,3. Green,4. Purple,5. Pink,6. Yellow,7. Gray,8. DarkBlue,9. DarkGreen,10. DarkPurple,11. DarkPink,12. DarkYellow"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1" sqref="L2:L1001" type="list">
+    <dataValidation sqref="L2:L1001" showErrorMessage="1" showDropDown="0" showInputMessage="1" allowBlank="0" type="list" operator="between">
       <formula1>"1. Shared,2. Not Shared"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
@@ -8035,17 +10333,17 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="2:67 A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="2:67 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.70703125" defaultRowHeight="14.4" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="8" width="9.66"/>
-    <col customWidth="1" max="2" min="2" style="8" width="23.35"/>
+    <col width="9.66" customWidth="1" style="8" min="1" max="1"/>
+    <col width="23.35" customWidth="1" style="8" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="14.4" r="1" s="9">
+    <row r="1" ht="14.4" customHeight="1" s="9">
       <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Date</t>
@@ -8057,7 +10355,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="2" s="9">
+    <row r="2" ht="14.4" customHeight="1" s="9">
       <c r="A2" s="14" t="inlineStr">
         <is>
           <t>1/1/2021</t>
@@ -8070,9 +10368,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
@@ -8084,17 +10382,17 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="2:67 A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="2:67 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.70703125" defaultRowHeight="14.4" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="8" width="17.56"/>
-    <col customWidth="1" max="3" min="2" style="8" width="25.79"/>
+    <col width="17.56" customWidth="1" style="8" min="1" max="1"/>
+    <col width="25.79" customWidth="1" style="8" min="2" max="3"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="14.4" r="1" s="9">
+    <row r="1" ht="14.4" customHeight="1" s="9">
       <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Name</t>
@@ -8111,7 +10409,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="2" s="9">
+    <row r="2" ht="14.4" customHeight="1" s="9">
       <c r="A2" s="8" t="inlineStr">
         <is>
           <t>Nodar Gelovani</t>
@@ -8128,7 +10426,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="3" s="9">
+    <row r="3" ht="14.4" customHeight="1" s="9">
       <c r="A3" s="8" t="inlineStr">
         <is>
           <t>Anastasia Ioseliani</t>
@@ -8145,7 +10443,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="4" s="9">
+    <row r="4" ht="14.4" customHeight="1" s="9">
       <c r="A4" s="8" t="inlineStr">
         <is>
           <t>Tamari Khardziani</t>
@@ -8162,7 +10460,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="5" s="9">
+    <row r="5" ht="14.4" customHeight="1" s="9">
       <c r="A5" s="8" t="inlineStr">
         <is>
           <t>Giorgi Gelovani</t>
@@ -8180,8 +10478,8 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
</xml_diff>